<commit_message>
clean up of unused files
</commit_message>
<xml_diff>
--- a/data/ROS_data_MEGA.xlsx
+++ b/data/ROS_data_MEGA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtalmy/Documents/code/metro_hastings/HOOH_dynamics/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidtalmy/Documents/code/metro_hastings/HOOH_dynamics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A95E00-D303-9B44-A2DA-BC0B75436B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292B97FB-95A6-9943-8EDA-005F0A2B7A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18200" yWindow="1240" windowWidth="22280" windowHeight="14020" xr2:uid="{82133392-E207-734F-898E-6135EBC32761}"/>
+    <workbookView xWindow="18200" yWindow="1240" windowWidth="22280" windowHeight="14020" firstSheet="3" activeTab="9" xr2:uid="{82133392-E207-734F-898E-6135EBC32761}"/>
   </bookViews>
   <sheets>
     <sheet name="Buffers_Morris_2011_f1c,d" sheetId="13" r:id="rId1"/>
@@ -958,7 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32616FE2-4A93-794C-A2B0-31ED69620F12}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2630,8 +2630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B1A5783-389B-0641-9BCF-F5B20268FA18}">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4083,7 +4083,7 @@
         <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D56" t="s">
         <v>32</v>
@@ -4118,7 +4118,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C57" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D57" t="s">
         <v>32</v>
@@ -4153,7 +4153,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C58" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D58" t="s">
         <v>32</v>
@@ -4188,7 +4188,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="C59" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D59" t="s">
         <v>32</v>
@@ -4223,7 +4223,7 @@
         <v>0.25</v>
       </c>
       <c r="C60" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D60" t="s">
         <v>32</v>
@@ -4258,7 +4258,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C61" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D61" t="s">
         <v>32</v>
@@ -4290,7 +4290,7 @@
         <v>0.375</v>
       </c>
       <c r="C62" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D62" t="s">
         <v>32</v>
@@ -4325,7 +4325,7 @@
         <v>0.5</v>
       </c>
       <c r="C63" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D63" t="s">
         <v>32</v>
@@ -4360,7 +4360,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C64" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D64" t="s">
         <v>32</v>
@@ -21110,7 +21110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248A308A-B8BF-B641-8603-CE5606553D5A}">
   <dimension ref="A1:J182"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A161" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -31923,17 +31923,12 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="L25:O25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="P45:Q45"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="L44:O44"/>
-    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="AD45:AE45"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AC16:AD16"/>
+    <mergeCell ref="AE16:AF16"/>
+    <mergeCell ref="AB44:AE44"/>
     <mergeCell ref="U16:V16"/>
     <mergeCell ref="T45:U45"/>
     <mergeCell ref="V45:W45"/>
@@ -31950,12 +31945,17 @@
     <mergeCell ref="AA26:AB26"/>
     <mergeCell ref="R45:S45"/>
     <mergeCell ref="AB45:AC45"/>
-    <mergeCell ref="AD45:AE45"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AC16:AD16"/>
-    <mergeCell ref="AE16:AF16"/>
-    <mergeCell ref="AB44:AE44"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="P45:Q45"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="L44:O44"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="K26:L26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>